<commit_message>
R script SRI + demographic + TOI + AOI
</commit_message>
<xml_diff>
--- a/01_studies/01_Laborstudie ProVisioNET/R script/sri coding/data/coding_sri_novice.xlsx
+++ b/01_studies/01_Laborstudie ProVisioNET/R script/sri coding/data/coding_sri_novice.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/505858402c07da9d/Dokumente/GitHub/Mandy-PhD/01_studies/01_Laborstudie ProVisioNET/R script/sri coding/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mk99feta\OneDrive\Dokumente\GitHub\Mandy-PhD\01_studies\01_Laborstudie ProVisioNET\R script\sri coding\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{BEC6D75F-56A4-41E5-B6F2-C33740C9160A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="14_{BEC6D75F-56A4-41E5-B6F2-C33740C9160A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{7E314719-6581-4C6B-B3F9-9FA243ECF3AB}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19428" windowHeight="10428" xr2:uid="{E076B5D5-D199-4D8E-A2C0-E3EC9D7FADC9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="24">
   <si>
     <t>whispering</t>
   </si>
@@ -493,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{403ECED8-55F4-4FC6-AC8C-3350BC92FAB2}">
-  <dimension ref="A1:F154"/>
+  <dimension ref="A1:F163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="H162" sqref="H162"/>
+    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="C165" sqref="C165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3547,6 +3547,186 @@
         <v>7</v>
       </c>
     </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A155" s="1">
+        <v>118</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D155" s="1">
+        <v>3</v>
+      </c>
+      <c r="E155" s="1">
+        <v>5</v>
+      </c>
+      <c r="F155" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A156" s="1">
+        <v>118</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D156" s="1">
+        <v>0</v>
+      </c>
+      <c r="E156" s="1">
+        <v>10</v>
+      </c>
+      <c r="F156" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A157" s="1">
+        <v>118</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D157" s="1">
+        <v>5</v>
+      </c>
+      <c r="E157" s="1">
+        <v>7</v>
+      </c>
+      <c r="F157" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A158" s="1">
+        <v>118</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D158" s="1">
+        <v>6</v>
+      </c>
+      <c r="E158" s="1">
+        <v>6</v>
+      </c>
+      <c r="F158" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A159" s="1">
+        <v>118</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D159" s="1">
+        <v>0</v>
+      </c>
+      <c r="E159" s="1">
+        <v>10</v>
+      </c>
+      <c r="F159" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A160" s="1">
+        <v>118</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D160" s="1">
+        <v>9</v>
+      </c>
+      <c r="E160" s="1">
+        <v>9</v>
+      </c>
+      <c r="F160" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A161" s="1">
+        <v>118</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D161" s="1">
+        <v>1</v>
+      </c>
+      <c r="E161" s="1">
+        <v>9</v>
+      </c>
+      <c r="F161" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A162" s="1">
+        <v>118</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D162" s="1">
+        <v>9</v>
+      </c>
+      <c r="E162" s="1">
+        <v>9</v>
+      </c>
+      <c r="F162" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A163" s="3">
+        <v>118</v>
+      </c>
+      <c r="B163" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C163" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D163" s="3">
+        <v>10</v>
+      </c>
+      <c r="E163" s="3">
+        <v>4</v>
+      </c>
+      <c r="F163" s="3">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>